<commit_message>
remove transfers, start fall 2012, check non-acad, adjust gpa with units
</commit_message>
<xml_diff>
--- a/major_divisions.xlsx
+++ b/major_divisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szy3\Documents\senior-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1679BC3-413E-478E-9A32-439CAD1AD5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A57C2D-C8B6-46AF-BC1A-B4A3A8FAF824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-150" yWindow="30" windowWidth="15165" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15165" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1057,7 +1057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="F208" sqref="F208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1369,15 +1369,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1420,18 +1420,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
       <c r="D43">
         <v>1</v>
       </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1843,18 +1843,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
       <c r="D85">
         <v>1</v>
       </c>
-      <c r="F85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2580,18 +2580,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
       <c r="C161">
         <v>1</v>
       </c>
-      <c r="F161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -2599,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -2607,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -2618,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -2629,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -2640,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -2648,12 +2645,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -2664,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -2675,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -2686,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -2697,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -2705,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2716,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -2727,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>

</xml_diff>

<commit_message>
fleshing out discussion and conclusion
</commit_message>
<xml_diff>
--- a/major_divisions.xlsx
+++ b/major_divisions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szy3\Documents\senior-thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiayang/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BB961B-33F8-4EE3-AF74-104F70546E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B2E3E3-E479-0F4E-A309-3DEF4C21C4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1056,20 +1056,20 @@
   <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E168" sqref="E168"/>
+      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B205" sqref="B205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -2986,15 +2986,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-      <c r="D205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>221</v>
       </c>

</xml_diff>